<commit_message>
Fix importer as sheet was missing a column
This includes the missing column in the xslx and updates the importer
also fix markdown of source url as join(" ") was not rendering correctly
</commit_message>
<xml_diff>
--- a/db/hmrc-plans.xlsx
+++ b/db/hmrc-plans.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="-20920" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="1 - PAYE" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <sheet name="22 - Trusts" sheetId="21" r:id="rId21"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">'1 - PAYE'!$D$29:$K$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">'1 - PAYE'!$D$29:$L$63</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3">'5 - Cross-cutting needs'!$D$15:$L$16</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4204" uniqueCount="1852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4205" uniqueCount="1853">
   <si>
     <t>Platform</t>
   </si>
@@ -6177,6 +6177,9 @@
   </si>
   <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>tasks</t>
   </si>
 </sst>
 </file>
@@ -8972,11 +8975,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="111" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="111" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="183">
+  <cellXfs count="190">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -9514,9 +9518,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="107" fillId="0" borderId="125" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -9526,9 +9527,34 @@
     <xf numFmtId="0" fontId="1" fillId="93" borderId="106" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="107" fillId="0" borderId="125" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="91" fillId="93" borderId="129" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="129" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="129" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="129" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="93" borderId="129" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="63" borderId="129" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -9858,13 +9884,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L66"/>
+  <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -9875,13 +9901,14 @@
     <col min="5" max="5" width="21" customWidth="1"/>
     <col min="6" max="6" width="38.1640625" customWidth="1"/>
     <col min="7" max="7" width="45.5" customWidth="1"/>
-    <col min="8" max="8" width="44.5" customWidth="1"/>
-    <col min="9" max="9" width="26.6640625" customWidth="1"/>
-    <col min="10" max="10" width="66.83203125" customWidth="1"/>
-    <col min="11" max="11" width="34.5" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" customWidth="1"/>
+    <col min="9" max="9" width="44.5" customWidth="1"/>
+    <col min="10" max="10" width="26.6640625" customWidth="1"/>
+    <col min="11" max="11" width="66.83203125" customWidth="1"/>
+    <col min="12" max="12" width="34.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="43" customHeight="1">
+    <row r="1" spans="1:13" ht="43" customHeight="1">
       <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
@@ -9903,23 +9930,26 @@
       <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="88" t="s">
+      <c r="H1" s="183" t="s">
+        <v>1852</v>
+      </c>
+      <c r="I1" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="88" t="s">
+      <c r="J1" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="88" t="s">
+      <c r="K1" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="88" t="s">
+      <c r="L1" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="M1" s="47" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="27" customHeight="1">
+    <row r="2" spans="1:13" ht="27" customHeight="1">
       <c r="A2" s="76" t="s">
         <v>13</v>
       </c>
@@ -9941,24 +9971,25 @@
       <c r="G2" s="148" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="172" t="s">
+      <c r="H2" s="184"/>
+      <c r="I2" s="172" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="81" t="s">
+      <c r="J2" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="172" t="s">
+      <c r="K2" s="172" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="172" t="s">
+      <c r="L2" s="172" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="157" t="str">
+      <c r="M2" s="157" t="str">
         <f>HYPERLINK("https://maslow.production.alphagov.co.uk/needs/100317", "100317")</f>
         <v>100317</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="27" customHeight="1">
+    <row r="3" spans="1:13" ht="27" customHeight="1">
       <c r="A3" s="76" t="s">
         <v>13</v>
       </c>
@@ -9980,22 +10011,23 @@
       <c r="G3" s="148" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="172" t="s">
+      <c r="H3" s="184"/>
+      <c r="I3" s="172" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="81" t="s">
+      <c r="J3" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="172"/>
-      <c r="K3" s="172" t="s">
+      <c r="K3" s="172"/>
+      <c r="L3" s="172" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="157" t="str">
+      <c r="M3" s="157" t="str">
         <f>HYPERLINK("https://maslow.production.alphagov.co.uk/needs/100317", "100317")</f>
         <v>100317</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="27" customHeight="1">
+    <row r="4" spans="1:13" ht="27" customHeight="1">
       <c r="A4" s="76" t="s">
         <v>13</v>
       </c>
@@ -10014,20 +10046,21 @@
       <c r="F4" s="148" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="182" t="s">
+      <c r="G4" s="181" t="s">
         <v>1851</v>
       </c>
-      <c r="H4" s="172" t="s">
+      <c r="H4" s="188"/>
+      <c r="I4" s="172" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="81" t="s">
+      <c r="J4" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="172"/>
       <c r="K4" s="172"/>
-      <c r="L4" s="157"/>
-    </row>
-    <row r="5" spans="1:12" ht="27" customHeight="1">
+      <c r="L4" s="172"/>
+      <c r="M4" s="157"/>
+    </row>
+    <row r="5" spans="1:13" ht="27" customHeight="1">
       <c r="A5" s="76" t="s">
         <v>13</v>
       </c>
@@ -10049,24 +10082,25 @@
       <c r="G5" s="148" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="172" t="s">
+      <c r="H5" s="184"/>
+      <c r="I5" s="172" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="81" t="s">
+      <c r="J5" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="J5" s="172" t="s">
+      <c r="K5" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="K5" s="172" t="s">
+      <c r="L5" s="172" t="s">
         <v>47</v>
       </c>
-      <c r="L5" s="157" t="str">
+      <c r="M5" s="157" t="str">
         <f>HYPERLINK("https://maslow.production.alphagov.co.uk/needs/100326", "100326")</f>
         <v>100326</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="27" customHeight="1">
+    <row r="6" spans="1:13" ht="27" customHeight="1">
       <c r="A6" s="76" t="s">
         <v>13</v>
       </c>
@@ -10088,24 +10122,25 @@
       <c r="G6" s="93" t="s">
         <v>51</v>
       </c>
-      <c r="H6" s="172" t="s">
+      <c r="H6" s="189"/>
+      <c r="I6" s="172" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="81" t="s">
+      <c r="J6" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="J6" s="29" t="s">
+      <c r="K6" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="K6" s="172" t="s">
+      <c r="L6" s="172" t="s">
         <v>55</v>
       </c>
-      <c r="L6" s="157" t="str">
+      <c r="M6" s="157" t="str">
         <f>HYPERLINK("https://maslow.production.alphagov.co.uk/needs/100252", "100252")</f>
         <v>100252</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="27" customHeight="1">
+    <row r="7" spans="1:13" ht="27" customHeight="1">
       <c r="A7" s="76" t="s">
         <v>13</v>
       </c>
@@ -10127,24 +10162,25 @@
       <c r="G7" s="148" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="172" t="s">
+      <c r="H7" s="184"/>
+      <c r="I7" s="172" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="81" t="s">
+      <c r="J7" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="172" t="s">
+      <c r="K7" s="172" t="s">
         <v>61</v>
       </c>
-      <c r="K7" s="179" t="s">
+      <c r="L7" s="182" t="s">
         <v>62</v>
       </c>
-      <c r="L7" s="157" t="str">
+      <c r="M7" s="157" t="str">
         <f>HYPERLINK("https://maslow.production.alphagov.co.uk/needs/100309", "100309")</f>
         <v>100309</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="27" customHeight="1">
+    <row r="8" spans="1:13" ht="27" customHeight="1">
       <c r="A8" s="76" t="s">
         <v>13</v>
       </c>
@@ -10166,20 +10202,21 @@
       <c r="G8" s="148" t="s">
         <v>66</v>
       </c>
-      <c r="H8" s="172" t="s">
+      <c r="H8" s="184"/>
+      <c r="I8" s="172" t="s">
         <v>67</v>
       </c>
-      <c r="I8" s="81" t="s">
+      <c r="J8" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="J8" s="172"/>
-      <c r="K8" s="179"/>
-      <c r="L8" s="157" t="str">
+      <c r="K8" s="172"/>
+      <c r="L8" s="182"/>
+      <c r="M8" s="157" t="str">
         <f>HYPERLINK("https://maslow.production.alphagov.co.uk/needs/100327", "100327")</f>
         <v>100327</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="27" customHeight="1">
+    <row r="9" spans="1:13" ht="27" customHeight="1">
       <c r="A9" s="76" t="s">
         <v>13</v>
       </c>
@@ -10199,24 +10236,25 @@
         <v>70</v>
       </c>
       <c r="G9" s="148"/>
-      <c r="H9" s="172" t="s">
+      <c r="H9" s="184"/>
+      <c r="I9" s="172" t="s">
         <v>71</v>
       </c>
-      <c r="I9" s="81" t="s">
+      <c r="J9" s="81" t="s">
         <v>72</v>
       </c>
-      <c r="J9" s="172" t="s">
+      <c r="K9" s="172" t="s">
         <v>73</v>
       </c>
-      <c r="K9" s="172" t="s">
+      <c r="L9" s="172" t="s">
         <v>74</v>
       </c>
-      <c r="L9" s="157" t="str">
+      <c r="M9" s="157" t="str">
         <f>HYPERLINK("https://maslow.production.alphagov.co.uk/needs/100329", "100329")</f>
         <v>100329</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="27" customHeight="1">
+    <row r="10" spans="1:13" ht="27" customHeight="1">
       <c r="A10" s="76" t="s">
         <v>13</v>
       </c>
@@ -10238,21 +10276,22 @@
       <c r="G10" s="148" t="s">
         <v>78</v>
       </c>
-      <c r="H10" s="172" t="s">
+      <c r="H10" s="184"/>
+      <c r="I10" s="172" t="s">
         <v>79</v>
       </c>
-      <c r="I10" s="81" t="s">
+      <c r="J10" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="J10" s="172" t="s">
+      <c r="K10" s="172" t="s">
         <v>81</v>
       </c>
-      <c r="K10" s="172" t="s">
+      <c r="L10" s="172" t="s">
         <v>82</v>
       </c>
-      <c r="L10" s="157"/>
-    </row>
-    <row r="11" spans="1:12" ht="27" customHeight="1">
+      <c r="M10" s="157"/>
+    </row>
+    <row r="11" spans="1:13" ht="27" customHeight="1">
       <c r="A11" s="76" t="s">
         <v>13</v>
       </c>
@@ -10274,13 +10313,14 @@
       <c r="G11" s="148" t="s">
         <v>86</v>
       </c>
-      <c r="H11" s="172"/>
-      <c r="I11" s="81"/>
-      <c r="J11" s="172"/>
+      <c r="H11" s="184"/>
+      <c r="I11" s="172"/>
+      <c r="J11" s="81"/>
       <c r="K11" s="172"/>
-      <c r="L11" s="157"/>
-    </row>
-    <row r="12" spans="1:12" ht="27" customHeight="1">
+      <c r="L11" s="172"/>
+      <c r="M11" s="157"/>
+    </row>
+    <row r="12" spans="1:13" ht="27" customHeight="1">
       <c r="A12" s="76" t="s">
         <v>13</v>
       </c>
@@ -10302,15 +10342,16 @@
       <c r="G12" s="148" t="s">
         <v>90</v>
       </c>
-      <c r="H12" s="172"/>
-      <c r="I12" s="81"/>
-      <c r="J12" s="172"/>
-      <c r="K12" s="172" t="s">
+      <c r="H12" s="184"/>
+      <c r="I12" s="172"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="172"/>
+      <c r="L12" s="172" t="s">
         <v>91</v>
       </c>
-      <c r="L12" s="157"/>
-    </row>
-    <row r="13" spans="1:12" ht="27" customHeight="1">
+      <c r="M12" s="157"/>
+    </row>
+    <row r="13" spans="1:13" ht="27" customHeight="1">
       <c r="A13" s="76" t="s">
         <v>13</v>
       </c>
@@ -10332,13 +10373,14 @@
       <c r="G13" s="148" t="s">
         <v>95</v>
       </c>
-      <c r="H13" s="172"/>
-      <c r="I13" s="81"/>
-      <c r="J13" s="172"/>
+      <c r="H13" s="184"/>
+      <c r="I13" s="172"/>
+      <c r="J13" s="81"/>
       <c r="K13" s="172"/>
-      <c r="L13" s="157"/>
-    </row>
-    <row r="14" spans="1:12" ht="27" customHeight="1">
+      <c r="L13" s="172"/>
+      <c r="M13" s="157"/>
+    </row>
+    <row r="14" spans="1:13" ht="27" customHeight="1">
       <c r="A14" s="76" t="s">
         <v>13</v>
       </c>
@@ -10360,13 +10402,14 @@
       <c r="G14" s="148" t="s">
         <v>99</v>
       </c>
-      <c r="H14" s="172"/>
-      <c r="I14" s="81"/>
-      <c r="J14" s="172"/>
+      <c r="H14" s="184"/>
+      <c r="I14" s="172"/>
+      <c r="J14" s="81"/>
       <c r="K14" s="172"/>
-      <c r="L14" s="157"/>
-    </row>
-    <row r="15" spans="1:12" ht="27" customHeight="1">
+      <c r="L14" s="172"/>
+      <c r="M14" s="157"/>
+    </row>
+    <row r="15" spans="1:13" ht="27" customHeight="1">
       <c r="A15" s="76" t="s">
         <v>13</v>
       </c>
@@ -10388,15 +10431,16 @@
       <c r="G15" s="148" t="s">
         <v>103</v>
       </c>
-      <c r="H15" s="172"/>
-      <c r="I15" s="81"/>
-      <c r="J15" s="172"/>
-      <c r="K15" s="172" t="s">
+      <c r="H15" s="184"/>
+      <c r="I15" s="172"/>
+      <c r="J15" s="81"/>
+      <c r="K15" s="172"/>
+      <c r="L15" s="172" t="s">
         <v>104</v>
       </c>
-      <c r="L15" s="157"/>
-    </row>
-    <row r="16" spans="1:12" ht="27" customHeight="1">
+      <c r="M15" s="157"/>
+    </row>
+    <row r="16" spans="1:13" ht="27" customHeight="1">
       <c r="A16" s="76" t="s">
         <v>13</v>
       </c>
@@ -10418,13 +10462,14 @@
       <c r="G16" s="148" t="s">
         <v>103</v>
       </c>
-      <c r="H16" s="172"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="172"/>
+      <c r="H16" s="184"/>
+      <c r="I16" s="172"/>
+      <c r="J16" s="81"/>
       <c r="K16" s="172"/>
-      <c r="L16" s="157"/>
-    </row>
-    <row r="17" spans="1:12" ht="27" customHeight="1">
+      <c r="L16" s="172"/>
+      <c r="M16" s="157"/>
+    </row>
+    <row r="17" spans="1:13" ht="27" customHeight="1">
       <c r="A17" s="76" t="s">
         <v>13</v>
       </c>
@@ -10446,15 +10491,16 @@
       <c r="G17" s="148" t="s">
         <v>111</v>
       </c>
-      <c r="H17" s="172"/>
-      <c r="I17" s="81"/>
-      <c r="J17" s="172"/>
-      <c r="K17" s="172" t="s">
+      <c r="H17" s="184"/>
+      <c r="I17" s="172"/>
+      <c r="J17" s="81"/>
+      <c r="K17" s="172"/>
+      <c r="L17" s="172" t="s">
         <v>112</v>
       </c>
-      <c r="L17" s="157"/>
-    </row>
-    <row r="18" spans="1:12" ht="27" customHeight="1">
+      <c r="M17" s="157"/>
+    </row>
+    <row r="18" spans="1:13" ht="27" customHeight="1">
       <c r="A18" s="76" t="s">
         <v>13</v>
       </c>
@@ -10476,15 +10522,16 @@
       <c r="G18" s="148" t="s">
         <v>116</v>
       </c>
-      <c r="H18" s="172"/>
-      <c r="I18" s="81"/>
-      <c r="J18" s="172"/>
-      <c r="K18" s="172" t="s">
+      <c r="H18" s="184"/>
+      <c r="I18" s="172"/>
+      <c r="J18" s="81"/>
+      <c r="K18" s="172"/>
+      <c r="L18" s="172" t="s">
         <v>117</v>
       </c>
-      <c r="L18" s="157"/>
-    </row>
-    <row r="19" spans="1:12" ht="27" customHeight="1">
+      <c r="M18" s="157"/>
+    </row>
+    <row r="19" spans="1:13" ht="27" customHeight="1">
       <c r="A19" s="76" t="s">
         <v>13</v>
       </c>
@@ -10506,15 +10553,16 @@
       <c r="G19" s="148" t="s">
         <v>121</v>
       </c>
-      <c r="H19" s="172"/>
-      <c r="I19" s="81"/>
-      <c r="J19" s="172"/>
-      <c r="K19" s="172" t="s">
+      <c r="H19" s="184"/>
+      <c r="I19" s="172"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="172"/>
+      <c r="L19" s="172" t="s">
         <v>122</v>
       </c>
-      <c r="L19" s="157"/>
-    </row>
-    <row r="20" spans="1:12" ht="27" customHeight="1">
+      <c r="M19" s="157"/>
+    </row>
+    <row r="20" spans="1:13" ht="27" customHeight="1">
       <c r="A20" s="76" t="s">
         <v>13</v>
       </c>
@@ -10536,15 +10584,16 @@
       <c r="G20" s="148" t="s">
         <v>126</v>
       </c>
-      <c r="H20" s="172"/>
-      <c r="I20" s="81"/>
-      <c r="J20" s="172"/>
-      <c r="K20" s="172" t="s">
+      <c r="H20" s="184"/>
+      <c r="I20" s="172"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="172"/>
+      <c r="L20" s="172" t="s">
         <v>127</v>
       </c>
-      <c r="L20" s="157"/>
-    </row>
-    <row r="21" spans="1:12" ht="27" customHeight="1">
+      <c r="M20" s="157"/>
+    </row>
+    <row r="21" spans="1:13" ht="27" customHeight="1">
       <c r="A21" s="76" t="s">
         <v>13</v>
       </c>
@@ -10566,15 +10615,16 @@
       <c r="G21" s="148" t="s">
         <v>90</v>
       </c>
-      <c r="H21" s="172"/>
-      <c r="I21" s="81"/>
-      <c r="J21" s="172"/>
-      <c r="K21" s="172" t="s">
+      <c r="H21" s="184"/>
+      <c r="I21" s="172"/>
+      <c r="J21" s="81"/>
+      <c r="K21" s="172"/>
+      <c r="L21" s="172" t="s">
         <v>131</v>
       </c>
-      <c r="L21" s="157"/>
-    </row>
-    <row r="22" spans="1:12" ht="27" customHeight="1">
+      <c r="M21" s="157"/>
+    </row>
+    <row r="22" spans="1:13" ht="27" customHeight="1">
       <c r="A22" s="76" t="s">
         <v>13</v>
       </c>
@@ -10596,24 +10646,25 @@
       <c r="G22" s="148" t="s">
         <v>135</v>
       </c>
-      <c r="H22" s="172" t="s">
+      <c r="H22" s="184"/>
+      <c r="I22" s="172" t="s">
         <v>136</v>
       </c>
-      <c r="I22" s="81" t="s">
+      <c r="J22" s="81" t="s">
         <v>72</v>
       </c>
-      <c r="J22" s="172" t="s">
+      <c r="K22" s="172" t="s">
         <v>137</v>
       </c>
-      <c r="K22" s="172" t="s">
+      <c r="L22" s="172" t="s">
         <v>138</v>
       </c>
-      <c r="L22" s="157" t="str">
+      <c r="M22" s="157" t="str">
         <f>HYPERLINK("https://maslow.production.alphagov.co.uk/needs/100328", "100328")</f>
         <v>100328</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="27" customHeight="1">
+    <row r="23" spans="1:13" ht="27" customHeight="1">
       <c r="A23" s="76" t="s">
         <v>13</v>
       </c>
@@ -10633,24 +10684,25 @@
         <v>141</v>
       </c>
       <c r="G23" s="148"/>
-      <c r="H23" s="172" t="s">
+      <c r="H23" s="184"/>
+      <c r="I23" s="172" t="s">
         <v>142</v>
       </c>
-      <c r="I23" s="81" t="s">
+      <c r="J23" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="J23" s="172" t="s">
+      <c r="K23" s="172" t="s">
         <v>143</v>
       </c>
-      <c r="K23" s="172" t="s">
+      <c r="L23" s="172" t="s">
         <v>144</v>
       </c>
-      <c r="L23" s="157" t="str">
+      <c r="M23" s="157" t="str">
         <f>HYPERLINK("https://maslow.production.alphagov.co.uk/needs/100330", "100330")</f>
         <v>100330</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="27" customHeight="1">
+    <row r="24" spans="1:13" ht="27" customHeight="1">
       <c r="A24" s="76" t="s">
         <v>13</v>
       </c>
@@ -10670,17 +10722,18 @@
         <v>147</v>
       </c>
       <c r="G24" s="148"/>
-      <c r="H24" s="172" t="s">
+      <c r="H24" s="184"/>
+      <c r="I24" s="172" t="s">
         <v>148</v>
       </c>
-      <c r="I24" s="81" t="s">
+      <c r="J24" s="81" t="s">
         <v>149</v>
       </c>
-      <c r="J24" s="172"/>
       <c r="K24" s="172"/>
-      <c r="L24" s="157"/>
-    </row>
-    <row r="25" spans="1:12" ht="27" customHeight="1">
+      <c r="L24" s="172"/>
+      <c r="M24" s="157"/>
+    </row>
+    <row r="25" spans="1:13" ht="27" customHeight="1">
       <c r="A25" s="76" t="s">
         <v>13</v>
       </c>
@@ -10700,22 +10753,23 @@
         <v>152</v>
       </c>
       <c r="G25" s="148"/>
-      <c r="H25" s="172" t="s">
+      <c r="H25" s="184"/>
+      <c r="I25" s="172" t="s">
         <v>153</v>
       </c>
-      <c r="I25" s="81" t="s">
+      <c r="J25" s="81" t="s">
         <v>72</v>
       </c>
-      <c r="J25" s="172"/>
-      <c r="K25" s="172" t="s">
+      <c r="K25" s="172"/>
+      <c r="L25" s="172" t="s">
         <v>154</v>
       </c>
-      <c r="L25" s="157" t="str">
+      <c r="M25" s="157" t="str">
         <f>HYPERLINK("https://maslow.production.alphagov.co.uk/needs/100294", "100294")</f>
         <v>100294</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="27" customHeight="1">
+    <row r="26" spans="1:13" ht="27" customHeight="1">
       <c r="A26" s="76" t="s">
         <v>13</v>
       </c>
@@ -10737,22 +10791,23 @@
       <c r="G26" s="148" t="s">
         <v>158</v>
       </c>
-      <c r="H26" s="172" t="s">
+      <c r="H26" s="184"/>
+      <c r="I26" s="172" t="s">
         <v>159</v>
       </c>
-      <c r="I26" s="81" t="s">
+      <c r="J26" s="81" t="s">
         <v>72</v>
       </c>
-      <c r="J26" s="172"/>
-      <c r="K26" s="172" t="s">
+      <c r="K26" s="172"/>
+      <c r="L26" s="172" t="s">
         <v>160</v>
       </c>
-      <c r="L26" s="157" t="str">
+      <c r="M26" s="157" t="str">
         <f>HYPERLINK("https://maslow.production.alphagov.co.uk/needs/100293", "100293")</f>
         <v>100293</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="27" customHeight="1">
+    <row r="27" spans="1:13" ht="27" customHeight="1">
       <c r="A27" s="76" t="s">
         <v>13</v>
       </c>
@@ -10774,22 +10829,23 @@
       <c r="G27" s="166" t="s">
         <v>164</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" s="185"/>
+      <c r="I27" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="J27" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3" t="s">
+      <c r="K27" s="3"/>
+      <c r="L27" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="L27" s="157" t="str">
+      <c r="M27" s="157" t="str">
         <f>HYPERLINK("https://maslow.production.alphagov.co.uk/needs/100295", "100295")</f>
         <v>100295</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="14.25" customHeight="1">
+    <row r="28" spans="1:13" ht="14.25" customHeight="1">
       <c r="A28" s="76" t="s">
         <v>13</v>
       </c>
@@ -10811,19 +10867,20 @@
       <c r="G28" s="148" t="s">
         <v>170</v>
       </c>
-      <c r="H28" s="172" t="s">
+      <c r="H28" s="184"/>
+      <c r="I28" s="172" t="s">
         <v>171</v>
       </c>
-      <c r="I28" s="81" t="s">
+      <c r="J28" s="81" t="s">
         <v>172</v>
       </c>
-      <c r="J28" s="81" t="s">
+      <c r="K28" s="81" t="s">
         <v>173</v>
       </c>
-      <c r="K28" s="81"/>
-      <c r="L28" s="157"/>
-    </row>
-    <row r="29" spans="1:12" ht="36.75" customHeight="1">
+      <c r="L28" s="81"/>
+      <c r="M28" s="157"/>
+    </row>
+    <row r="29" spans="1:13" ht="36.75" customHeight="1">
       <c r="A29" s="76" t="s">
         <v>13</v>
       </c>
@@ -10845,19 +10902,20 @@
       <c r="G29" s="148" t="s">
         <v>177</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H29" s="184"/>
+      <c r="I29" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="J29" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="J29" s="3" t="s">
+      <c r="K29" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="K29" s="172"/>
-      <c r="L29" s="157"/>
-    </row>
-    <row r="30" spans="1:12" ht="36.75" customHeight="1">
+      <c r="L29" s="172"/>
+      <c r="M29" s="157"/>
+    </row>
+    <row r="30" spans="1:13" ht="36.75" customHeight="1">
       <c r="A30" s="76" t="s">
         <v>13</v>
       </c>
@@ -10879,17 +10937,18 @@
       <c r="G30" s="148" t="s">
         <v>184</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="H30" s="184"/>
+      <c r="I30" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="I30" s="3" t="s">
+      <c r="J30" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="J30" s="3"/>
-      <c r="K30" s="172"/>
-      <c r="L30" s="157"/>
-    </row>
-    <row r="31" spans="1:12" ht="36.75" customHeight="1">
+      <c r="K30" s="3"/>
+      <c r="L30" s="172"/>
+      <c r="M30" s="157"/>
+    </row>
+    <row r="31" spans="1:13" ht="36.75" customHeight="1">
       <c r="A31" s="76" t="s">
         <v>13</v>
       </c>
@@ -10909,19 +10968,20 @@
         <v>189</v>
       </c>
       <c r="G31" s="148"/>
-      <c r="H31" s="3" t="s">
+      <c r="H31" s="184"/>
+      <c r="I31" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="I31" s="148" t="s">
+      <c r="J31" s="148" t="s">
         <v>191</v>
       </c>
-      <c r="J31" s="3"/>
-      <c r="K31" s="172" t="s">
+      <c r="K31" s="3"/>
+      <c r="L31" s="172" t="s">
         <v>192</v>
       </c>
-      <c r="L31" s="157"/>
-    </row>
-    <row r="32" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M31" s="157"/>
+    </row>
+    <row r="32" spans="1:13" ht="36.75" customHeight="1">
       <c r="A32" s="76" t="s">
         <v>13</v>
       </c>
@@ -10943,17 +11003,18 @@
       <c r="G32" s="148" t="s">
         <v>197</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="H32" s="184"/>
+      <c r="I32" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="I32" s="3" t="s">
+      <c r="J32" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="J32" s="3"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="157"/>
-    </row>
-    <row r="33" spans="1:12" ht="36.75" customHeight="1">
+      <c r="K32" s="3"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="157"/>
+    </row>
+    <row r="33" spans="1:13" ht="36.75" customHeight="1">
       <c r="A33" s="76" t="s">
         <v>13</v>
       </c>
@@ -10975,21 +11036,22 @@
       <c r="G33" s="148" t="s">
         <v>202</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="H33" s="184"/>
+      <c r="I33" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="J33" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="J33" s="3" t="s">
+      <c r="K33" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="K33" s="172" t="s">
+      <c r="L33" s="172" t="s">
         <v>206</v>
       </c>
-      <c r="L33" s="157"/>
-    </row>
-    <row r="34" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M33" s="157"/>
+    </row>
+    <row r="34" spans="1:13" ht="36.75" customHeight="1">
       <c r="A34" s="76" t="s">
         <v>13</v>
       </c>
@@ -11011,19 +11073,20 @@
       <c r="G34" s="166" t="s">
         <v>210</v>
       </c>
-      <c r="H34" s="29" t="s">
+      <c r="H34" s="185"/>
+      <c r="I34" s="29" t="s">
         <v>211</v>
       </c>
-      <c r="I34" s="3" t="s">
+      <c r="J34" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3" t="s">
+      <c r="K34" s="3"/>
+      <c r="L34" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="L34" s="157"/>
-    </row>
-    <row r="35" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M34" s="157"/>
+    </row>
+    <row r="35" spans="1:13" ht="36.75" customHeight="1">
       <c r="A35" s="76" t="s">
         <v>13</v>
       </c>
@@ -11045,19 +11108,20 @@
       <c r="G35" s="166" t="s">
         <v>217</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="H35" s="185"/>
+      <c r="I35" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="I35" s="3" t="s">
+      <c r="J35" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="J35" s="3"/>
       <c r="K35" s="3"/>
-      <c r="L35" s="157" t="s">
+      <c r="L35" s="3"/>
+      <c r="M35" s="157" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="36.75" customHeight="1">
+    <row r="36" spans="1:13" ht="36.75" customHeight="1">
       <c r="A36" s="76" t="s">
         <v>221</v>
       </c>
@@ -11079,17 +11143,18 @@
       <c r="G36" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="H36" s="172"/>
-      <c r="I36" s="76" t="s">
+      <c r="H36" s="186"/>
+      <c r="I36" s="172"/>
+      <c r="J36" s="76" t="s">
         <v>227</v>
       </c>
-      <c r="J36" s="172"/>
-      <c r="K36" s="172" t="s">
+      <c r="K36" s="172"/>
+      <c r="L36" s="172" t="s">
         <v>228</v>
       </c>
-      <c r="L36" s="157"/>
-    </row>
-    <row r="37" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M36" s="157"/>
+    </row>
+    <row r="37" spans="1:13" ht="36.75" customHeight="1">
       <c r="A37" s="76" t="s">
         <v>221</v>
       </c>
@@ -11111,17 +11176,18 @@
       <c r="G37" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="H37" s="172"/>
-      <c r="I37" s="76" t="s">
+      <c r="H37" s="186"/>
+      <c r="I37" s="172"/>
+      <c r="J37" s="76" t="s">
         <v>232</v>
       </c>
-      <c r="J37" s="172"/>
-      <c r="K37" s="172" t="s">
+      <c r="K37" s="172"/>
+      <c r="L37" s="172" t="s">
         <v>228</v>
       </c>
-      <c r="L37" s="157"/>
-    </row>
-    <row r="38" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M37" s="157"/>
+    </row>
+    <row r="38" spans="1:13" ht="36.75" customHeight="1">
       <c r="A38" s="76" t="s">
         <v>221</v>
       </c>
@@ -11143,17 +11209,18 @@
       <c r="G38" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="H38" s="172"/>
-      <c r="I38" s="76" t="s">
+      <c r="H38" s="186"/>
+      <c r="I38" s="172"/>
+      <c r="J38" s="76" t="s">
         <v>227</v>
       </c>
-      <c r="J38" s="172"/>
-      <c r="K38" s="172" t="s">
+      <c r="K38" s="172"/>
+      <c r="L38" s="172" t="s">
         <v>228</v>
       </c>
-      <c r="L38" s="157"/>
-    </row>
-    <row r="39" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M38" s="157"/>
+    </row>
+    <row r="39" spans="1:13" ht="36.75" customHeight="1">
       <c r="A39" s="76" t="s">
         <v>221</v>
       </c>
@@ -11175,17 +11242,18 @@
       <c r="G39" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="H39" s="172"/>
-      <c r="I39" s="76" t="s">
+      <c r="H39" s="186"/>
+      <c r="I39" s="172"/>
+      <c r="J39" s="76" t="s">
         <v>232</v>
       </c>
-      <c r="J39" s="172"/>
-      <c r="K39" s="172" t="s">
+      <c r="K39" s="172"/>
+      <c r="L39" s="172" t="s">
         <v>228</v>
       </c>
-      <c r="L39" s="157"/>
-    </row>
-    <row r="40" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M39" s="157"/>
+    </row>
+    <row r="40" spans="1:13" ht="36.75" customHeight="1">
       <c r="A40" s="76" t="s">
         <v>221</v>
       </c>
@@ -11207,17 +11275,18 @@
       <c r="G40" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="H40" s="172"/>
-      <c r="I40" s="76" t="s">
+      <c r="H40" s="186"/>
+      <c r="I40" s="172"/>
+      <c r="J40" s="76" t="s">
         <v>227</v>
       </c>
-      <c r="J40" s="172"/>
-      <c r="K40" s="172" t="s">
+      <c r="K40" s="172"/>
+      <c r="L40" s="172" t="s">
         <v>228</v>
       </c>
-      <c r="L40" s="157"/>
-    </row>
-    <row r="41" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M40" s="157"/>
+    </row>
+    <row r="41" spans="1:13" ht="36.75" customHeight="1">
       <c r="A41" s="76" t="s">
         <v>221</v>
       </c>
@@ -11239,17 +11308,18 @@
       <c r="G41" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="H41" s="172"/>
-      <c r="I41" s="76" t="s">
+      <c r="H41" s="186"/>
+      <c r="I41" s="172"/>
+      <c r="J41" s="76" t="s">
         <v>242</v>
       </c>
-      <c r="J41" s="172"/>
-      <c r="K41" s="172" t="s">
+      <c r="K41" s="172"/>
+      <c r="L41" s="172" t="s">
         <v>228</v>
       </c>
-      <c r="L41" s="157"/>
-    </row>
-    <row r="42" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M41" s="157"/>
+    </row>
+    <row r="42" spans="1:13" ht="36.75" customHeight="1">
       <c r="A42" s="76" t="s">
         <v>221</v>
       </c>
@@ -11271,17 +11341,18 @@
       <c r="G42" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H42" s="3"/>
-      <c r="I42" s="76" t="s">
+      <c r="H42" s="186"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="76" t="s">
         <v>232</v>
       </c>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3" t="s">
+      <c r="K42" s="3"/>
+      <c r="L42" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L42" s="157"/>
-    </row>
-    <row r="43" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M42" s="157"/>
+    </row>
+    <row r="43" spans="1:13" ht="36.75" customHeight="1">
       <c r="A43" s="76" t="s">
         <v>221</v>
       </c>
@@ -11303,17 +11374,18 @@
       <c r="G43" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H43" s="3"/>
-      <c r="I43" s="76" t="s">
+      <c r="H43" s="186"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="76" t="s">
         <v>227</v>
       </c>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3" t="s">
+      <c r="K43" s="3"/>
+      <c r="L43" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L43" s="157"/>
-    </row>
-    <row r="44" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M43" s="157"/>
+    </row>
+    <row r="44" spans="1:13" ht="36.75" customHeight="1">
       <c r="A44" s="76" t="s">
         <v>221</v>
       </c>
@@ -11335,17 +11407,18 @@
       <c r="G44" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H44" s="3"/>
-      <c r="I44" s="76" t="s">
+      <c r="H44" s="186"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="76" t="s">
         <v>232</v>
       </c>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3" t="s">
+      <c r="K44" s="3"/>
+      <c r="L44" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L44" s="157"/>
-    </row>
-    <row r="45" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M44" s="157"/>
+    </row>
+    <row r="45" spans="1:13" ht="36.75" customHeight="1">
       <c r="A45" s="76" t="s">
         <v>221</v>
       </c>
@@ -11367,17 +11440,18 @@
       <c r="G45" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H45" s="3"/>
-      <c r="I45" s="76" t="s">
+      <c r="H45" s="186"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="76" t="s">
         <v>252</v>
       </c>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3" t="s">
+      <c r="K45" s="3"/>
+      <c r="L45" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L45" s="157"/>
-    </row>
-    <row r="46" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M45" s="157"/>
+    </row>
+    <row r="46" spans="1:13" ht="36.75" customHeight="1">
       <c r="A46" s="76" t="s">
         <v>221</v>
       </c>
@@ -11399,17 +11473,18 @@
       <c r="G46" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="H46" s="3"/>
-      <c r="I46" s="76" t="s">
+      <c r="H46" s="186"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="76" t="s">
         <v>242</v>
       </c>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3" t="s">
+      <c r="K46" s="3"/>
+      <c r="L46" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L46" s="157"/>
-    </row>
-    <row r="47" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M46" s="157"/>
+    </row>
+    <row r="47" spans="1:13" ht="36.75" customHeight="1">
       <c r="A47" s="76" t="s">
         <v>221</v>
       </c>
@@ -11431,17 +11506,18 @@
       <c r="G47" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="H47" s="3"/>
-      <c r="I47" s="76" t="s">
+      <c r="H47" s="186"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="76" t="s">
         <v>242</v>
       </c>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3" t="s">
+      <c r="K47" s="3"/>
+      <c r="L47" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L47" s="157"/>
-    </row>
-    <row r="48" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M47" s="157"/>
+    </row>
+    <row r="48" spans="1:13" ht="36.75" customHeight="1">
       <c r="A48" s="76" t="s">
         <v>221</v>
       </c>
@@ -11463,17 +11539,18 @@
       <c r="G48" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H48" s="3"/>
-      <c r="I48" s="76" t="s">
+      <c r="H48" s="186"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="76" t="s">
         <v>252</v>
       </c>
-      <c r="J48" s="3"/>
-      <c r="K48" s="127" t="s">
+      <c r="K48" s="3"/>
+      <c r="L48" s="127" t="s">
         <v>259</v>
       </c>
-      <c r="L48" s="157"/>
-    </row>
-    <row r="49" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M48" s="157"/>
+    </row>
+    <row r="49" spans="1:13" ht="36.75" customHeight="1">
       <c r="A49" s="76" t="s">
         <v>221</v>
       </c>
@@ -11495,17 +11572,18 @@
       <c r="G49" s="70" t="s">
         <v>245</v>
       </c>
-      <c r="H49" s="3"/>
-      <c r="I49" s="76" t="s">
+      <c r="H49" s="187"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3" t="s">
+      <c r="K49" s="3"/>
+      <c r="L49" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L49" s="157"/>
-    </row>
-    <row r="50" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M49" s="157"/>
+    </row>
+    <row r="50" spans="1:13" ht="36.75" customHeight="1">
       <c r="A50" s="76" t="s">
         <v>221</v>
       </c>
@@ -11527,17 +11605,18 @@
       <c r="G50" s="70" t="s">
         <v>245</v>
       </c>
-      <c r="H50" s="3"/>
-      <c r="I50" s="76" t="s">
+      <c r="H50" s="187"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3" t="s">
+      <c r="K50" s="3"/>
+      <c r="L50" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L50" s="157"/>
-    </row>
-    <row r="51" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M50" s="157"/>
+    </row>
+    <row r="51" spans="1:13" ht="36.75" customHeight="1">
       <c r="A51" s="76" t="s">
         <v>221</v>
       </c>
@@ -11559,17 +11638,18 @@
       <c r="G51" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H51" s="3"/>
-      <c r="I51" s="76" t="s">
+      <c r="H51" s="186"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="76" t="s">
         <v>252</v>
       </c>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3" t="s">
+      <c r="K51" s="3"/>
+      <c r="L51" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L51" s="157"/>
-    </row>
-    <row r="52" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M51" s="157"/>
+    </row>
+    <row r="52" spans="1:13" ht="36.75" customHeight="1">
       <c r="A52" s="76" t="s">
         <v>221</v>
       </c>
@@ -11591,17 +11671,18 @@
       <c r="G52" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H52" s="3"/>
-      <c r="I52" s="76" t="s">
+      <c r="H52" s="186"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="76" t="s">
         <v>232</v>
       </c>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3" t="s">
+      <c r="K52" s="3"/>
+      <c r="L52" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L52" s="157"/>
-    </row>
-    <row r="53" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M52" s="157"/>
+    </row>
+    <row r="53" spans="1:13" ht="36.75" customHeight="1">
       <c r="A53" s="76" t="s">
         <v>221</v>
       </c>
@@ -11623,17 +11704,18 @@
       <c r="G53" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H53" s="3"/>
-      <c r="I53" s="76" t="s">
+      <c r="H53" s="186"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="76" t="s">
         <v>242</v>
       </c>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3" t="s">
+      <c r="K53" s="3"/>
+      <c r="L53" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L53" s="157"/>
-    </row>
-    <row r="54" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M53" s="157"/>
+    </row>
+    <row r="54" spans="1:13" ht="36.75" customHeight="1">
       <c r="A54" s="29" t="s">
         <v>221</v>
       </c>
@@ -11655,17 +11737,18 @@
       <c r="G54" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="H54" s="3"/>
-      <c r="I54" s="76" t="s">
+      <c r="H54" s="186"/>
+      <c r="I54" s="3"/>
+      <c r="J54" s="76" t="s">
         <v>242</v>
       </c>
-      <c r="J54" s="3"/>
-      <c r="K54" s="3" t="s">
+      <c r="K54" s="3"/>
+      <c r="L54" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L54" s="157"/>
-    </row>
-    <row r="55" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M54" s="157"/>
+    </row>
+    <row r="55" spans="1:13" ht="36.75" customHeight="1">
       <c r="A55" s="29" t="s">
         <v>221</v>
       </c>
@@ -11687,17 +11770,18 @@
       <c r="G55" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="H55" s="3"/>
-      <c r="I55" s="76" t="s">
+      <c r="H55" s="186"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="76" t="s">
         <v>242</v>
       </c>
-      <c r="J55" s="3"/>
-      <c r="K55" s="3" t="s">
+      <c r="K55" s="3"/>
+      <c r="L55" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L55" s="157"/>
-    </row>
-    <row r="56" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M55" s="157"/>
+    </row>
+    <row r="56" spans="1:13" ht="36.75" customHeight="1">
       <c r="A56" s="29" t="s">
         <v>221</v>
       </c>
@@ -11719,17 +11803,18 @@
       <c r="G56" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H56" s="3"/>
-      <c r="I56" s="76" t="s">
+      <c r="H56" s="186"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="76" t="s">
         <v>232</v>
       </c>
-      <c r="J56" s="3"/>
-      <c r="K56" s="3" t="s">
+      <c r="K56" s="3"/>
+      <c r="L56" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L56" s="157"/>
-    </row>
-    <row r="57" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M56" s="157"/>
+    </row>
+    <row r="57" spans="1:13" ht="36.75" customHeight="1">
       <c r="A57" s="29" t="s">
         <v>221</v>
       </c>
@@ -11751,17 +11836,18 @@
       <c r="G57" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H57" s="3"/>
-      <c r="I57" s="76" t="s">
+      <c r="H57" s="186"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="76" t="s">
         <v>232</v>
       </c>
-      <c r="J57" s="3"/>
-      <c r="K57" s="3" t="s">
+      <c r="K57" s="3"/>
+      <c r="L57" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L57" s="157"/>
-    </row>
-    <row r="58" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M57" s="157"/>
+    </row>
+    <row r="58" spans="1:13" ht="36.75" customHeight="1">
       <c r="A58" s="29" t="s">
         <v>221</v>
       </c>
@@ -11783,17 +11869,18 @@
       <c r="G58" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H58" s="3"/>
-      <c r="I58" s="76" t="s">
+      <c r="H58" s="186"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="76" t="s">
         <v>232</v>
       </c>
-      <c r="J58" s="3"/>
-      <c r="K58" s="3" t="s">
+      <c r="K58" s="3"/>
+      <c r="L58" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L58" s="157"/>
-    </row>
-    <row r="59" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M58" s="157"/>
+    </row>
+    <row r="59" spans="1:13" ht="36.75" customHeight="1">
       <c r="A59" s="29" t="s">
         <v>221</v>
       </c>
@@ -11815,17 +11902,18 @@
       <c r="G59" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H59" s="3"/>
-      <c r="I59" s="76" t="s">
+      <c r="H59" s="186"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="76" t="s">
         <v>232</v>
       </c>
-      <c r="J59" s="3"/>
-      <c r="K59" s="3" t="s">
+      <c r="K59" s="3"/>
+      <c r="L59" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L59" s="157"/>
-    </row>
-    <row r="60" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M59" s="157"/>
+    </row>
+    <row r="60" spans="1:13" ht="36.75" customHeight="1">
       <c r="A60" s="29" t="s">
         <v>221</v>
       </c>
@@ -11847,17 +11935,18 @@
       <c r="G60" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H60" s="3"/>
-      <c r="I60" s="76" t="s">
+      <c r="H60" s="186"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="76" t="s">
         <v>227</v>
       </c>
-      <c r="J60" s="3"/>
-      <c r="K60" s="3" t="s">
+      <c r="K60" s="3"/>
+      <c r="L60" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L60" s="157"/>
-    </row>
-    <row r="61" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M60" s="157"/>
+    </row>
+    <row r="61" spans="1:13" ht="36.75" customHeight="1">
       <c r="A61" s="29" t="s">
         <v>221</v>
       </c>
@@ -11879,17 +11968,18 @@
       <c r="G61" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H61" s="3"/>
-      <c r="I61" s="76" t="s">
+      <c r="H61" s="186"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="76" t="s">
         <v>227</v>
       </c>
-      <c r="J61" s="3"/>
-      <c r="K61" s="3" t="s">
+      <c r="K61" s="3"/>
+      <c r="L61" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L61" s="157"/>
-    </row>
-    <row r="62" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M61" s="157"/>
+    </row>
+    <row r="62" spans="1:13" ht="36.75" customHeight="1">
       <c r="A62" s="29" t="s">
         <v>221</v>
       </c>
@@ -11911,17 +12001,18 @@
       <c r="G62" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H62" s="3"/>
-      <c r="I62" s="76" t="s">
+      <c r="H62" s="186"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="76" t="s">
         <v>227</v>
       </c>
-      <c r="J62" s="3"/>
-      <c r="K62" s="3" t="s">
+      <c r="K62" s="3"/>
+      <c r="L62" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L62" s="157"/>
-    </row>
-    <row r="63" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M62" s="157"/>
+    </row>
+    <row r="63" spans="1:13" ht="36.75" customHeight="1">
       <c r="A63" s="29" t="s">
         <v>221</v>
       </c>
@@ -11943,17 +12034,18 @@
       <c r="G63" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H63" s="3"/>
-      <c r="I63" s="3" t="s">
+      <c r="H63" s="186"/>
+      <c r="I63" s="3"/>
+      <c r="J63" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="J63" s="3"/>
-      <c r="K63" s="127" t="s">
+      <c r="K63" s="3"/>
+      <c r="L63" s="127" t="s">
         <v>293</v>
       </c>
-      <c r="L63" s="157"/>
-    </row>
-    <row r="64" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M63" s="157"/>
+    </row>
+    <row r="64" spans="1:13" ht="36.75" customHeight="1">
       <c r="A64" s="29" t="s">
         <v>221</v>
       </c>
@@ -11975,15 +12067,16 @@
       <c r="G64" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H64" s="3"/>
-      <c r="I64" s="3" t="s">
+      <c r="H64" s="186"/>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="J64" s="3"/>
-      <c r="K64" s="127"/>
-      <c r="L64" s="157"/>
-    </row>
-    <row r="65" spans="1:12" ht="36.75" customHeight="1">
+      <c r="K64" s="3"/>
+      <c r="L64" s="127"/>
+      <c r="M64" s="157"/>
+    </row>
+    <row r="65" spans="1:13" ht="36.75" customHeight="1">
       <c r="A65" s="29" t="s">
         <v>221</v>
       </c>
@@ -12005,15 +12098,16 @@
       <c r="G65" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H65" s="3"/>
-      <c r="I65" s="3" t="s">
+      <c r="H65" s="186"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="J65" s="3"/>
-      <c r="K65" s="127"/>
-      <c r="L65" s="157"/>
-    </row>
-    <row r="66" spans="1:12" ht="36.75" customHeight="1">
+      <c r="K65" s="3"/>
+      <c r="L65" s="127"/>
+      <c r="M65" s="157"/>
+    </row>
+    <row r="66" spans="1:13" ht="36.75" customHeight="1">
       <c r="A66" s="29" t="s">
         <v>221</v>
       </c>
@@ -12035,17 +12129,18 @@
       <c r="G66" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H66" s="3"/>
-      <c r="I66" s="3" t="s">
+      <c r="H66" s="186"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="J66" s="3"/>
-      <c r="K66" s="127"/>
-      <c r="L66" s="157"/>
+      <c r="K66" s="3"/>
+      <c r="L66" s="127"/>
+      <c r="M66" s="157"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -15120,7 +15215,7 @@
       <c r="C11" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="181" t="s">
+      <c r="D11" s="180" t="s">
         <v>1850</v>
       </c>
       <c r="E11" s="33" t="s">
@@ -15145,7 +15240,7 @@
       <c r="C12" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="181" t="s">
+      <c r="D12" s="180" t="s">
         <v>1850</v>
       </c>
       <c r="E12" s="33" t="s">
@@ -15170,7 +15265,7 @@
       <c r="C13" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="181" t="s">
+      <c r="D13" s="180" t="s">
         <v>1850</v>
       </c>
       <c r="E13" s="33" t="s">
@@ -15195,7 +15290,7 @@
       <c r="C14" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="181" t="s">
+      <c r="D14" s="180" t="s">
         <v>1850</v>
       </c>
       <c r="E14" s="33" t="s">
@@ -15220,7 +15315,7 @@
       <c r="C15" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="181" t="s">
+      <c r="D15" s="180" t="s">
         <v>1850</v>
       </c>
       <c r="E15" s="33" t="s">
@@ -15243,7 +15338,7 @@
       <c r="C16" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="181" t="s">
+      <c r="D16" s="180" t="s">
         <v>1850</v>
       </c>
       <c r="E16" s="33" t="s">
@@ -15267,7 +15362,7 @@
       <c r="C17" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="181" t="s">
+      <c r="D17" s="180" t="s">
         <v>1850</v>
       </c>
       <c r="E17" s="33" t="s">
@@ -15293,7 +15388,7 @@
       <c r="C18" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="181" t="s">
+      <c r="D18" s="180" t="s">
         <v>1850</v>
       </c>
       <c r="E18" s="33" t="s">
@@ -15317,7 +15412,7 @@
       <c r="C19" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="181" t="s">
+      <c r="D19" s="180" t="s">
         <v>1850</v>
       </c>
       <c r="E19" s="33" t="s">
@@ -15343,7 +15438,7 @@
       <c r="C20" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="181" t="s">
+      <c r="D20" s="180" t="s">
         <v>1850</v>
       </c>
       <c r="E20" s="4" t="s">
@@ -15369,7 +15464,7 @@
       <c r="C21" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="181" t="s">
+      <c r="D21" s="180" t="s">
         <v>1850</v>
       </c>
       <c r="E21" s="4" t="s">
@@ -15395,7 +15490,7 @@
       <c r="C22" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="181" t="s">
+      <c r="D22" s="180" t="s">
         <v>1850</v>
       </c>
       <c r="E22" s="4" t="s">
@@ -15421,7 +15516,7 @@
       <c r="C23" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="181" t="s">
+      <c r="D23" s="180" t="s">
         <v>1850</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -15447,7 +15542,7 @@
       <c r="C24" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="181" t="s">
+      <c r="D24" s="180" t="s">
         <v>1850</v>
       </c>
       <c r="E24" s="4" t="s">
@@ -15473,7 +15568,7 @@
       <c r="C25" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="181" t="s">
+      <c r="D25" s="180" t="s">
         <v>1850</v>
       </c>
       <c r="E25" s="4" t="s">
@@ -15499,7 +15594,7 @@
       <c r="C26" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="181" t="s">
+      <c r="D26" s="180" t="s">
         <v>1850</v>
       </c>
       <c r="E26" s="4" t="s">
@@ -20625,7 +20720,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -25834,10 +25929,10 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -26447,7 +26542,7 @@
         <v>778</v>
       </c>
       <c r="F16" s="164"/>
-      <c r="G16" s="180" t="s">
+      <c r="G16" s="179" t="s">
         <v>1850</v>
       </c>
       <c r="H16" s="144"/>
@@ -26474,7 +26569,7 @@
         <v>686</v>
       </c>
       <c r="F17" s="164"/>
-      <c r="G17" s="180" t="s">
+      <c r="G17" s="179" t="s">
         <v>1850</v>
       </c>
       <c r="H17" s="144"/>
@@ -26501,7 +26596,7 @@
         <v>694</v>
       </c>
       <c r="F18" s="164"/>
-      <c r="G18" s="180" t="s">
+      <c r="G18" s="179" t="s">
         <v>1850</v>
       </c>
       <c r="H18" s="144"/>
@@ -26528,7 +26623,7 @@
         <v>779</v>
       </c>
       <c r="F19" s="164"/>
-      <c r="G19" s="180" t="s">
+      <c r="G19" s="179" t="s">
         <v>1850</v>
       </c>
       <c r="H19" s="144"/>
@@ -26555,7 +26650,7 @@
         <v>780</v>
       </c>
       <c r="F20" s="164"/>
-      <c r="G20" s="180" t="s">
+      <c r="G20" s="179" t="s">
         <v>1850</v>
       </c>
       <c r="H20" s="144"/>
@@ -26582,7 +26677,7 @@
         <v>710</v>
       </c>
       <c r="F21" s="164"/>
-      <c r="G21" s="180" t="s">
+      <c r="G21" s="179" t="s">
         <v>1850</v>
       </c>
       <c r="H21" s="144"/>
@@ -26609,7 +26704,7 @@
         <v>781</v>
       </c>
       <c r="F22" s="164"/>
-      <c r="G22" s="180" t="s">
+      <c r="G22" s="179" t="s">
         <v>1850</v>
       </c>
       <c r="H22" s="144"/>
@@ -26636,7 +26731,7 @@
         <v>734</v>
       </c>
       <c r="F23" s="164"/>
-      <c r="G23" s="180" t="s">
+      <c r="G23" s="179" t="s">
         <v>1850</v>
       </c>
       <c r="H23" s="144"/>
@@ -26663,7 +26758,7 @@
         <v>782</v>
       </c>
       <c r="F24" s="164"/>
-      <c r="G24" s="180" t="s">
+      <c r="G24" s="179" t="s">
         <v>1850</v>
       </c>
       <c r="H24" s="144" t="s">
@@ -28252,9 +28347,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>